<commit_message>
Added Onion Fest data and refactored CreateTourneyData to scale better with more tournaments.
</commit_message>
<xml_diff>
--- a/Stats/2022_LogJam_Stats.xlsx
+++ b/Stats/2022_LogJam_Stats.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="41">
   <si>
     <t>DPP</t>
   </si>
@@ -71,73 +71,76 @@
     <t>TAA</t>
   </si>
   <si>
-    <t>Adam P</t>
+    <t>Adam Parler</t>
   </si>
   <si>
-    <t>Alan A</t>
+    <t>Alan Albrecht</t>
   </si>
   <si>
-    <t>Kevin B</t>
+    <t>Kevin Baar</t>
   </si>
   <si>
-    <t>Jordan H</t>
+    <t>Jordan Harvey</t>
   </si>
   <si>
-    <t>Kaylynn J</t>
+    <t>Kaylynn Jay</t>
   </si>
   <si>
     <t>Michaela F</t>
   </si>
   <si>
-    <t>Sam J</t>
+    <t>Sam Johnson</t>
   </si>
   <si>
-    <t>Harry S</t>
+    <t>Harry Stone</t>
   </si>
   <si>
-    <t>Shawn C</t>
+    <t>Shawn Campbell</t>
   </si>
   <si>
-    <t>Trevor K</t>
+    <t>Trevor Kilgannnon</t>
   </si>
   <si>
-    <t>Annie F</t>
+    <t>Annie Fyfeyfe</t>
   </si>
   <si>
-    <t>Erica K</t>
+    <t>Erica Kilgannon</t>
   </si>
   <si>
-    <t>Loni K</t>
+    <t>Loni Kringle</t>
   </si>
   <si>
-    <t>Sam D</t>
+    <t>Sam Diedesch</t>
   </si>
   <si>
-    <t>Kevin F</t>
+    <t>Kevin Fiedler</t>
   </si>
   <si>
-    <t>Zac C</t>
+    <t>Zac Carter</t>
   </si>
   <si>
-    <t>Josh S</t>
+    <t>Josh Sokolowski</t>
   </si>
   <si>
-    <t>Kira M</t>
+    <t>Kira Murray</t>
   </si>
   <si>
-    <t>Sarah L</t>
+    <t>Sarah Leichty</t>
   </si>
   <si>
-    <t>Jason F</t>
+    <t>Jason Fuller</t>
   </si>
   <si>
-    <t>Jeremy T</t>
+    <t>Jeremy Tucknies</t>
   </si>
   <si>
-    <t>Denny P</t>
+    <t>Denny Porter</t>
   </si>
   <si>
-    <t>Jasmine W</t>
+    <t>Annie Fyfe</t>
+  </si>
+  <si>
+    <t>Jasmine Woo</t>
   </si>
   <si>
     <t>Total</t>
@@ -498,7 +501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1089,13 +1092,13 @@
         <v>26</v>
       </c>
       <c r="B12">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1116,25 +1119,25 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>0.125</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="M12">
-        <v>-3.36</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="O12">
-        <v>0.6363636363636364</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <v>0.71</v>
+        <v>-0.57</v>
       </c>
       <c r="Q12">
-        <v>-2.66</v>
+        <v>-0.57</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1725,131 +1728,184 @@
         <v>38</v>
       </c>
       <c r="B24">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>23</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>0.07692307692307693</v>
+      </c>
+      <c r="M24">
+        <v>-3.36</v>
+      </c>
+      <c r="N24">
+        <v>7</v>
+      </c>
+      <c r="O24">
+        <v>0.7</v>
+      </c>
+      <c r="P24">
+        <v>1.28</v>
+      </c>
+      <c r="Q24">
+        <v>-2.09</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25">
         <v>9</v>
       </c>
-      <c r="C24">
+      <c r="C25">
         <v>6</v>
       </c>
-      <c r="D24">
+      <c r="D25">
         <v>15</v>
       </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24">
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
         <v>0.1111111111111111</v>
       </c>
-      <c r="M24">
+      <c r="M25">
         <v>-1.24</v>
       </c>
-      <c r="N24">
-        <v>3</v>
-      </c>
-      <c r="O24">
+      <c r="N25">
+        <v>3</v>
+      </c>
+      <c r="O25">
         <v>0.5</v>
       </c>
-      <c r="P24">
+      <c r="P25">
         <v>-0.47</v>
       </c>
-      <c r="Q24">
+      <c r="Q25">
         <v>-1.71</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="1"/>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
+    <row r="26" spans="1:17">
+      <c r="A26" s="1"/>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
         <v>-0</v>
       </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-      <c r="P25">
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
         <v>-0</v>
       </c>
-      <c r="Q25">
+      <c r="Q26">
         <v>-0</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26">
+    <row r="27" spans="1:17">
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27">
         <v>58.71428571428572</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>74.85714285714286</v>
       </c>
-      <c r="D26">
+      <c r="D27">
         <v>133.5714285714286</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>55</v>
       </c>
-      <c r="G26">
+      <c r="G27">
         <v>55</v>
       </c>
-      <c r="I26">
+      <c r="I27">
         <v>110</v>
       </c>
-      <c r="K26">
+      <c r="K27">
         <v>17</v>
       </c>
-      <c r="N26">
+      <c r="N27">
         <v>42</v>
       </c>
     </row>
@@ -3084,7 +3140,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>6</v>
@@ -3388,7 +3444,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -4130,7 +4186,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -4342,7 +4398,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>12</v>
@@ -4646,7 +4702,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -5282,7 +5338,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -5600,7 +5656,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>8</v>
@@ -6169,7 +6225,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -6487,7 +6543,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B17">
         <v>3</v>
@@ -6803,7 +6859,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B23">
         <v>10.85714285714286</v>
@@ -7107,7 +7163,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>4</v>
@@ -7849,7 +7905,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -8061,7 +8117,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>10</v>
@@ -9213,7 +9269,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22">
         <v>8.857142857142858</v>
@@ -10153,7 +10209,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -10259,7 +10315,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -10471,7 +10527,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>3</v>

</xml_diff>